<commit_message>
Correcao do wait request no top level do sync ip + driver C para o sync no Nios
</commit_message>
<xml_diff>
--- a/FPGA_Developments/Sync/doc/sync_registers.xlsx
+++ b/FPGA_Developments/Sync/doc/sync_registers.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos\nsee\simucam_fpga\FPGA_Developments\Sync\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cassio\repo_simucam\SimuCam_Development\FPGA_Developments\Sync\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9375"/>
   </bookViews>
   <sheets>
     <sheet name="sync_regs" sheetId="1" r:id="rId1"/>
@@ -1162,24 +1162,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" customWidth="1"/>
-    <col min="5" max="5" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="57.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="57.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:11" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:11" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>33</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>0</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1263,7 +1263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1286,7 +1286,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1309,7 +1309,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1332,7 +1332,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -1343,7 +1343,7 @@
       <c r="H8" s="59"/>
       <c r="I8" s="21"/>
     </row>
-    <row r="9" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="51"/>
       <c r="B9" s="52" t="s">
         <v>89</v>
@@ -1356,7 +1356,7 @@
       <c r="H9" s="60"/>
       <c r="I9" s="55"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>1</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1406,7 +1406,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1429,7 +1429,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1440,7 +1440,7 @@
       <c r="H13" s="57"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>2</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1490,7 +1490,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1513,7 +1513,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -1524,7 +1524,7 @@
       <c r="H17" s="57"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>3</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1574,7 +1574,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1597,7 +1597,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -1608,7 +1608,7 @@
       <c r="H21" s="59"/>
       <c r="I21" s="27"/>
     </row>
-    <row r="22" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="28"/>
       <c r="B22" s="23" t="s">
         <v>42</v>
@@ -1621,7 +1621,7 @@
       <c r="H22" s="61"/>
       <c r="I22" s="26"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>4</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <v>5</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
         <v>6</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>7</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>8</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -1789,7 +1789,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -1812,7 +1812,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="29"/>
       <c r="B30" s="30"/>
       <c r="C30" s="30"/>
@@ -1823,7 +1823,7 @@
       <c r="H30" s="59"/>
       <c r="I30" s="31"/>
     </row>
-    <row r="31" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22">
         <v>9</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18"/>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
@@ -1863,7 +1863,7 @@
       <c r="H32" s="59"/>
       <c r="I32" s="27"/>
     </row>
-    <row r="33" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22">
         <v>10</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="37"/>
       <c r="B34" s="38"/>
       <c r="C34" s="38"/>
@@ -1915,7 +1915,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1938,7 +1938,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1961,7 +1961,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1984,7 +1984,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2007,7 +2007,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2053,7 +2053,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2076,7 +2076,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2099,7 +2099,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2122,7 +2122,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2145,7 +2145,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2168,7 +2168,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2191,7 +2191,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2214,7 +2214,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="9"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -2237,7 +2237,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="4:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revisao geral do sync ip e complementos no driver C para o Nios
</commit_message>
<xml_diff>
--- a/FPGA_Developments/Sync/doc/sync_registers.xlsx
+++ b/FPGA_Developments/Sync/doc/sync_registers.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cassio\repo_simucam\SimuCam_Development\FPGA_Developments\Sync\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos\nsee\simucam_fpga\FPGA_Developments\Sync\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="sync_regs" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>Bit Field Position</t>
   </si>
   <si>
-    <t>Internal/External_n status bit</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>Reset</t>
   </si>
   <si>
-    <t>Int_ext_n</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -321,6 +315,12 @@
   </si>
   <si>
     <t>Reset Value</t>
+  </si>
+  <si>
+    <t>Extn_int</t>
+  </si>
+  <si>
+    <t>External_n / Internal sync status bit</t>
   </si>
 </sst>
 </file>
@@ -1162,26 +1162,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="57.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="57.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:11" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:11" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>0</v>
@@ -1202,30 +1202,30 @@
         <v>4</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K2" s="50" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="14">
         <v>0</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
@@ -1237,41 +1237,41 @@
         <v>0</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F4" s="41">
         <v>7</v>
       </c>
       <c r="G4" s="41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" s="58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I4" s="42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F5" s="2">
         <v>8</v>
@@ -1283,18 +1283,18 @@
         <v>0</v>
       </c>
       <c r="I5" s="33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F6" s="2">
         <v>8</v>
@@ -1306,18 +1306,18 @@
         <v>0</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="2">
         <v>8</v>
@@ -1329,10 +1329,10 @@
         <v>0</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -1343,10 +1343,10 @@
       <c r="H8" s="59"/>
       <c r="I8" s="21"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A9" s="51"/>
       <c r="B9" s="52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C9" s="53"/>
       <c r="D9" s="54"/>
@@ -1356,42 +1356,42 @@
       <c r="H9" s="60"/>
       <c r="I9" s="55"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="17">
         <v>1</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E10" s="41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F10" s="41">
         <v>30</v>
       </c>
       <c r="G10" s="41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H10" s="58"/>
       <c r="I10" s="43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -1403,18 +1403,18 @@
         <v>0</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
@@ -1426,10 +1426,10 @@
         <v>0</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1440,65 +1440,65 @@
       <c r="H13" s="57"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>2</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F14" s="41">
         <v>30</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H14" s="58"/>
       <c r="I14" s="43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="57">
+        <v>0</v>
+      </c>
+      <c r="I15" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="F15" s="2">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" s="57">
-        <v>0</v>
-      </c>
-      <c r="I15" s="56" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
@@ -1510,10 +1510,10 @@
         <v>0</v>
       </c>
       <c r="I16" s="56" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -1524,42 +1524,42 @@
       <c r="H17" s="57"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="17">
         <v>3</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F18" s="41">
         <v>30</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H18" s="58"/>
       <c r="I18" s="43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" s="2">
         <v>1</v>
@@ -1571,18 +1571,18 @@
         <v>0</v>
       </c>
       <c r="I19" s="34" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
@@ -1594,10 +1594,10 @@
         <v>0</v>
       </c>
       <c r="I20" s="34" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -1608,10 +1608,10 @@
       <c r="H21" s="59"/>
       <c r="I21" s="27"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A22" s="28"/>
       <c r="B22" s="23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="24"/>
@@ -1621,24 +1621,24 @@
       <c r="H22" s="61"/>
       <c r="I22" s="26"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="17">
         <v>4</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>6</v>
@@ -1647,27 +1647,27 @@
         <v>0</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="17">
         <v>5</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>6</v>
@@ -1676,27 +1676,27 @@
         <v>0</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="17">
         <v>6</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>6</v>
@@ -1705,27 +1705,27 @@
         <v>0</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="17">
         <v>7</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>6</v>
@@ -1734,47 +1734,47 @@
         <v>0</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="17">
         <v>8</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E27" s="41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F27" s="41">
         <v>23</v>
       </c>
       <c r="G27" s="41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H27" s="58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I27" s="44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="17"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
       <c r="D28" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F28" s="2">
         <v>1</v>
@@ -1786,18 +1786,18 @@
         <v>0</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
       <c r="D29" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F29" s="2">
         <v>8</v>
@@ -1809,10 +1809,10 @@
         <v>0</v>
       </c>
       <c r="I29" s="49" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="29"/>
       <c r="B30" s="30"/>
       <c r="C30" s="30"/>
@@ -1823,24 +1823,24 @@
       <c r="H30" s="59"/>
       <c r="I30" s="31"/>
     </row>
-    <row r="31" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A31" s="22">
         <v>9</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C31" s="23" t="s">
         <v>5</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G31" s="25" t="s">
         <v>6</v>
@@ -1849,10 +1849,10 @@
         <v>0</v>
       </c>
       <c r="I31" s="32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18"/>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
@@ -1863,21 +1863,21 @@
       <c r="H32" s="59"/>
       <c r="I32" s="27"/>
     </row>
-    <row r="33" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A33" s="22">
         <v>10</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C33" s="23" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="F33" s="25">
         <v>1</v>
@@ -1889,41 +1889,41 @@
         <v>0</v>
       </c>
       <c r="I33" s="36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="37"/>
       <c r="B34" s="38"/>
       <c r="C34" s="38"/>
       <c r="D34" s="45" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E34" s="46" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F34" s="46">
         <v>11</v>
       </c>
       <c r="G34" s="46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H34" s="62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I34" s="47" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F35" s="2">
         <v>1</v>
@@ -1935,18 +1935,18 @@
         <v>0</v>
       </c>
       <c r="I35" s="33" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F36" s="2">
         <v>1</v>
@@ -1958,18 +1958,18 @@
         <v>0</v>
       </c>
       <c r="I36" s="33" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F37" s="2">
         <v>1</v>
@@ -1981,18 +1981,18 @@
         <v>0</v>
       </c>
       <c r="I37" s="33" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F38" s="2">
         <v>1</v>
@@ -2004,41 +2004,41 @@
         <v>0</v>
       </c>
       <c r="I38" s="33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E39" s="41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F39" s="41">
         <v>7</v>
       </c>
       <c r="G39" s="41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H39" s="58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I39" s="48" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F40" s="2">
         <v>1</v>
@@ -2050,18 +2050,18 @@
         <v>0</v>
       </c>
       <c r="I40" s="33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F41" s="2">
         <v>1</v>
@@ -2073,18 +2073,18 @@
         <v>0</v>
       </c>
       <c r="I41" s="33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F42" s="2">
         <v>1</v>
@@ -2096,18 +2096,18 @@
         <v>0</v>
       </c>
       <c r="I42" s="33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="7"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F43" s="2">
         <v>1</v>
@@ -2119,18 +2119,18 @@
         <v>0</v>
       </c>
       <c r="I43" s="33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="7"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F44" s="2">
         <v>1</v>
@@ -2142,18 +2142,18 @@
         <v>0</v>
       </c>
       <c r="I44" s="33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="7"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F45" s="2">
         <v>1</v>
@@ -2165,18 +2165,18 @@
         <v>0</v>
       </c>
       <c r="I45" s="33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F46" s="2">
         <v>1</v>
@@ -2188,18 +2188,18 @@
         <v>0</v>
       </c>
       <c r="I46" s="33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="7"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F47" s="2">
         <v>1</v>
@@ -2211,18 +2211,18 @@
         <v>0</v>
       </c>
       <c r="I47" s="33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
       <c r="D48" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F48" s="10">
         <v>1</v>
@@ -2234,10 +2234,10 @@
         <v>0</v>
       </c>
       <c r="I48" s="35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D49" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ensaios finais de validacao do sync ip - update no driver nios
</commit_message>
<xml_diff>
--- a/FPGA_Developments/Sync/doc/sync_registers.xlsx
+++ b/FPGA_Developments/Sync/doc/sync_registers.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos\nsee\simucam_fpga\FPGA_Developments\Sync\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cassio\repo_simucam\SimuCam_Development\FPGA_Developments\Sync\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9375"/>
   </bookViews>
   <sheets>
     <sheet name="sync_regs" sheetId="1" r:id="rId1"/>
@@ -1160,26 +1160,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K49"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="57.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="57.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:11" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>31</v>
       </c>
@@ -1207,11 +1210,8 @@
       <c r="I2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="50" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>0</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1263,7 +1263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1286,7 +1286,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1309,7 +1309,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1332,7 +1332,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -1343,7 +1343,7 @@
       <c r="H8" s="59"/>
       <c r="I8" s="21"/>
     </row>
-    <row r="9" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="51"/>
       <c r="B9" s="52" t="s">
         <v>87</v>
@@ -1356,7 +1356,7 @@
       <c r="H9" s="60"/>
       <c r="I9" s="55"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>1</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1406,7 +1406,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1429,7 +1429,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1440,7 +1440,7 @@
       <c r="H13" s="57"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>2</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1490,7 +1490,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1513,7 +1513,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -1524,7 +1524,7 @@
       <c r="H17" s="57"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>3</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1574,7 +1574,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1597,7 +1597,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -1608,7 +1608,7 @@
       <c r="H21" s="59"/>
       <c r="I21" s="27"/>
     </row>
-    <row r="22" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="28"/>
       <c r="B22" s="23" t="s">
         <v>40</v>
@@ -1621,7 +1621,7 @@
       <c r="H22" s="61"/>
       <c r="I22" s="26"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>4</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <v>5</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
         <v>6</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>7</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>8</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -1789,7 +1789,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -1812,7 +1812,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="29"/>
       <c r="B30" s="30"/>
       <c r="C30" s="30"/>
@@ -1823,7 +1823,7 @@
       <c r="H30" s="59"/>
       <c r="I30" s="31"/>
     </row>
-    <row r="31" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22">
         <v>9</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18"/>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
@@ -1863,7 +1863,7 @@
       <c r="H32" s="59"/>
       <c r="I32" s="27"/>
     </row>
-    <row r="33" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22">
         <v>10</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="37"/>
       <c r="B34" s="38"/>
       <c r="C34" s="38"/>
@@ -1915,7 +1915,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1938,7 +1938,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1961,7 +1961,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1984,7 +1984,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2007,7 +2007,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2030,7 +2030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2053,7 +2053,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2076,7 +2076,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2099,7 +2099,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2122,7 +2122,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2145,7 +2145,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2168,7 +2168,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2191,7 +2191,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2214,7 +2214,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="9"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -2237,12 +2237,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="4:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="50" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="B2:G48"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="61" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>